<commit_message>
Added features : - Stable coins prices - Format on floats - Dexscreener link - Transaction link - Update dex_parameters.xlsx with new datas - Gas limit set automatically (just had to not specify gas limit...)
Issues :
- trisolaris low liquidity on stablecoin display wrong prics on terminal

Next evolutions :
- Add a functionality to swap token for tokens (TOP PRIORITY)
- Connection with websockets to increase speed
- Add a functionality to approve token you bought and sell
- Add a functionality to set a take profit and stop loss
- Add other DEXs and blockchains
</commit_message>
<xml_diff>
--- a/dex_parameters.xlsx
+++ b/dex_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/new/PycharmProjects/DeFi Cheat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/new/PycharmProjects/BuyTokenOnDex/v1.0.1/buyTokenOnDex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8534833-D9CB-D440-899F-EE517355516A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E7D100-7E50-4145-AAC1-C86A48E65224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{88565959-7D13-C549-BFB5-A27F108CA62F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{88565959-7D13-C549-BFB5-A27F108CA62F}"/>
   </bookViews>
   <sheets>
     <sheet name="dex_parameters" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
   <si>
     <t>Dex</t>
   </si>
@@ -190,6 +190,156 @@
   </si>
   <si>
     <t>[{"type":"constructor","stateMutability":"nonpayable","inputs":[{"type":"address","name":"_factory","internalType":"address"},{"type":"address","name":"_WETH","internalType":"address"}]},{"type":"function","stateMutability":"view","outputs":[{"type":"address","name":"","internalType":"address"}],"name":"WETH","inputs":[]},{"type":"function","stateMutability":"nonpayable","outputs":[{"type":"uint256","name":"amountA","internalType":"uint256"},{"type":"uint256","name":"amountB","internalType":"uint256"},{"type":"uint256","name":"liquidity","internalType":"uint256"}],"name":"addLiquidity","inputs":[{"type":"address","name":"tokenA","internalType":"address"},{"type":"address","name":"tokenB","internalType":"address"},{"type":"uint256","name":"amountADesired","internalType":"uint256"},{"type":"uint256","name":"amountBDesired","internalType":"uint256"},{"type":"uint256","name":"amountAMin","internalType":"uint256"},{"type":"uint256","name":"amountBMin","internalType":"uint256"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"payable","outputs":[{"type":"uint256","name":"amountToken","internalType":"uint256"},{"type":"uint256","name":"amountETH","internalType":"uint256"},{"type":"uint256","name":"liquidity","internalType":"uint256"}],"name":"addLiquidityETH","inputs":[{"type":"address","name":"token","internalType":"address"},{"type":"uint256","name":"amountTokenDesired","internalType":"uint256"},{"type":"uint256","name":"amountTokenMin","internalType":"uint256"},{"type":"uint256","name":"amountETHMin","internalType":"uint256"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"view","outputs":[{"type":"address","name":"","internalType":"address"}],"name":"factory","inputs":[]},{"type":"function","stateMutability":"pure","outputs":[{"type":"uint256","name":"amountIn","internalType":"uint256"}],"name":"getAmountIn","inputs":[{"type":"uint256","name":"amountOut","internalType":"uint256"},{"type":"uint256","name":"reserveIn","internalType":"uint256"},{"type":"uint256","name":"reserveOut","internalType":"uint256"}]},{"type":"function","stateMutability":"pure","outputs":[{"type":"uint256","name":"amountOut","internalType":"uint256"}],"name":"getAmountOut","inputs":[{"type":"uint256","name":"amountIn","internalType":"uint256"},{"type":"uint256","name":"reserveIn","internalType":"uint256"},{"type":"uint256","name":"reserveOut","internalType":"uint256"}]},{"type":"function","stateMutability":"view","outputs":[{"type":"uint256[]","name":"amounts","internalType":"uint256[]"}],"name":"getAmountsIn","inputs":[{"type":"uint256","name":"amountOut","internalType":"uint256"},{"type":"address[]","name":"path","internalType":"address[]"}]},{"type":"function","stateMutability":"view","outputs":[{"type":"uint256[]","name":"amounts","internalType":"uint256[]"}],"name":"getAmountsOut","inputs":[{"type":"uint256","name":"amountIn","internalType":"uint256"},{"type":"address[]","name":"path","internalType":"address[]"}]},{"type":"function","stateMutability":"pure","outputs":[{"type":"uint256","name":"amountB","internalType":"uint256"}],"name":"quote","inputs":[{"type":"uint256","name":"amountA","internalType":"uint256"},{"type":"uint256","name":"reserveA","internalType":"uint256"},{"type":"uint256","name":"reserveB","internalType":"uint256"}]},{"type":"function","stateMutability":"nonpayable","outputs":[{"type":"uint256","name":"amountA","internalType":"uint256"},{"type":"uint256","name":"amountB","internalType":"uint256"}],"name":"removeLiquidity","inputs":[{"type":"address","name":"tokenA","internalType":"address"},{"type":"address","name":"tokenB","internalType":"address"},{"type":"uint256","name":"liquidity","internalType":"uint256"},{"type":"uint256","name":"amountAMin","internalType":"uint256"},{"type":"uint256","name":"amountBMin","internalType":"uint256"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"nonpayable","outputs":[{"type":"uint256","name":"amountToken","internalType":"uint256"},{"type":"uint256","name":"amountETH","internalType":"uint256"}],"name":"removeLiquidityETH","inputs":[{"type":"address","name":"token","internalType":"address"},{"type":"uint256","name":"liquidity","internalType":"uint256"},{"type":"uint256","name":"amountTokenMin","internalType":"uint256"},{"type":"uint256","name":"amountETHMin","internalType":"uint256"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"nonpayable","outputs":[{"type":"uint256","name":"amountETH","internalType":"uint256"}],"name":"removeLiquidityETHSupportingFeeOnTransferTokens","inputs":[{"type":"address","name":"token","internalType":"address"},{"type":"uint256","name":"liquidity","internalType":"uint256"},{"type":"uint256","name":"amountTokenMin","internalType":"uint256"},{"type":"uint256","name":"amountETHMin","internalType":"uint256"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"nonpayable","outputs":[{"type":"uint256","name":"amountToken","internalType":"uint256"},{"type":"uint256","name":"amountETH","internalType":"uint256"}],"name":"removeLiquidityETHWithPermit","inputs":[{"type":"address","name":"token","internalType":"address"},{"type":"uint256","name":"liquidity","internalType":"uint256"},{"type":"uint256","name":"amountTokenMin","internalType":"uint256"},{"type":"uint256","name":"amountETHMin","internalType":"uint256"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"},{"type":"bool","name":"approveMax","internalType":"bool"},{"type":"uint8","name":"v","internalType":"uint8"},{"type":"bytes32","name":"r","internalType":"bytes32"},{"type":"bytes32","name":"s","internalType":"bytes32"}]},{"type":"function","stateMutability":"nonpayable","outputs":[{"type":"uint256","name":"amountETH","internalType":"uint256"}],"name":"removeLiquidityETHWithPermitSupportingFeeOnTransferTokens","inputs":[{"type":"address","name":"token","internalType":"address"},{"type":"uint256","name":"liquidity","internalType":"uint256"},{"type":"uint256","name":"amountTokenMin","internalType":"uint256"},{"type":"uint256","name":"amountETHMin","internalType":"uint256"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"},{"type":"bool","name":"approveMax","internalType":"bool"},{"type":"uint8","name":"v","internalType":"uint8"},{"type":"bytes32","name":"r","internalType":"bytes32"},{"type":"bytes32","name":"s","internalType":"bytes32"}]},{"type":"function","stateMutability":"nonpayable","outputs":[{"type":"uint256","name":"amountA","internalType":"uint256"},{"type":"uint256","name":"amountB","internalType":"uint256"}],"name":"removeLiquidityWithPermit","inputs":[{"type":"address","name":"tokenA","internalType":"address"},{"type":"address","name":"tokenB","internalType":"address"},{"type":"uint256","name":"liquidity","internalType":"uint256"},{"type":"uint256","name":"amountAMin","internalType":"uint256"},{"type":"uint256","name":"amountBMin","internalType":"uint256"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"},{"type":"bool","name":"approveMax","internalType":"bool"},{"type":"uint8","name":"v","internalType":"uint8"},{"type":"bytes32","name":"r","internalType":"bytes32"},{"type":"bytes32","name":"s","internalType":"bytes32"}]},{"type":"function","stateMutability":"payable","outputs":[{"type":"uint256[]","name":"amounts","internalType":"uint256[]"}],"name":"swapETHForExactTokens","inputs":[{"type":"uint256","name":"amountOut","internalType":"uint256"},{"type":"address[]","name":"path","internalType":"address[]"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"payable","outputs":[{"type":"uint256[]","name":"amounts","internalType":"uint256[]"}],"name":"swapExactETHForTokens","inputs":[{"type":"uint256","name":"amountOutMin","internalType":"uint256"},{"type":"address[]","name":"path","internalType":"address[]"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"payable","outputs":[],"name":"swapExactETHForTokensSupportingFeeOnTransferTokens","inputs":[{"type":"uint256","name":"amountOutMin","internalType":"uint256"},{"type":"address[]","name":"path","internalType":"address[]"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"nonpayable","outputs":[{"type":"uint256[]","name":"amounts","internalType":"uint256[]"}],"name":"swapExactTokensForETH","inputs":[{"type":"uint256","name":"amountIn","internalType":"uint256"},{"type":"uint256","name":"amountOutMin","internalType":"uint256"},{"type":"address[]","name":"path","internalType":"address[]"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"nonpayable","outputs":[],"name":"swapExactTokensForETHSupportingFeeOnTransferTokens","inputs":[{"type":"uint256","name":"amountIn","internalType":"uint256"},{"type":"uint256","name":"amountOutMin","internalType":"uint256"},{"type":"address[]","name":"path","internalType":"address[]"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"nonpayable","outputs":[{"type":"uint256[]","name":"amounts","internalType":"uint256[]"}],"name":"swapExactTokensForTokens","inputs":[{"type":"uint256","name":"amountIn","internalType":"uint256"},{"type":"uint256","name":"amountOutMin","internalType":"uint256"},{"type":"address[]","name":"path","internalType":"address[]"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"nonpayable","outputs":[],"name":"swapExactTokensForTokensSupportingFeeOnTransferTokens","inputs":[{"type":"uint256","name":"amountIn","internalType":"uint256"},{"type":"uint256","name":"amountOutMin","internalType":"uint256"},{"type":"address[]","name":"path","internalType":"address[]"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"nonpayable","outputs":[{"type":"uint256[]","name":"amounts","internalType":"uint256[]"}],"name":"swapTokensForExactETH","inputs":[{"type":"uint256","name":"amountOut","internalType":"uint256"},{"type":"uint256","name":"amountInMax","internalType":"uint256"},{"type":"address[]","name":"path","internalType":"address[]"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"function","stateMutability":"nonpayable","outputs":[{"type":"uint256[]","name":"amounts","internalType":"uint256[]"}],"name":"swapTokensForExactTokens","inputs":[{"type":"uint256","name":"amountOut","internalType":"uint256"},{"type":"uint256","name":"amountInMax","internalType":"uint256"},{"type":"address[]","name":"path","internalType":"address[]"},{"type":"address","name":"to","internalType":"address"},{"type":"uint256","name":"deadline","internalType":"uint256"}]},{"type":"receive","stateMutability":"payable"}]</t>
+  </si>
+  <si>
+    <t>0xA7D7079b0FEaD91F3e65f86E8915Cb59c1a4C664</t>
+  </si>
+  <si>
+    <t>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"chainId","type":"uint256"}],"name":"AddSupportedChainId","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"contractAddress","type":"address"},{"indexed":false,"internalType":"uint256","name":"supplyIncrement","type":"uint256"}],"name":"AddSwapToken","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"newBridgeRoleAddress","type":"address"}],"name":"MigrateBridgeRole","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"},{"indexed":false,"internalType":"address","name":"feeAddress","type":"address"},{"indexed":false,"internalType":"uint256","name":"feeAmount","type":"uint256"},{"indexed":false,"internalType":"bytes32","name":"originTxId","type":"bytes32"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"contractAddress","type":"address"},{"indexed":false,"internalType":"uint256","name":"supplyDecrement","type":"uint256"}],"name":"RemoveSwapToken","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"token","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"chainId","type":"uint256"}],"name":"Unwrap","type":"event"},{"inputs":[{"internalType":"uint256","name":"chainId","type":"uint256"}],"name":"addSupportedChainId","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"contractAddress","type":"address"},{"internalType":"uint256","name":"supplyIncrement","type":"uint256"}],"name":"addSwapToken","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"burn","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"burnFrom","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"chainIds","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"subtractedValue","type":"uint256"}],"name":"decreaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"addedValue","type":"uint256"}],"name":"increaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newBridgeRoleAddress","type":"address"}],"name":"migrateBridgeRole","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"},{"internalType":"address","name":"feeAddress","type":"address"},{"internalType":"uint256","name":"feeAmount","type":"uint256"},{"internalType":"bytes32","name":"originTxId","type":"bytes32"}],"name":"mint","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"contractAddress","type":"address"},{"internalType":"uint256","name":"supplyDecrement","type":"uint256"}],"name":"removeSwapToken","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"token","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"swap","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"token","type":"address"}],"name":"swapSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"sender","type":"address"},{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"},{"internalType":"uint256","name":"chainId","type":"uint256"}],"name":"unwrap","outputs":[],"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t>0x04068DA6C83AFCFA0e13ba15A6696662335D5B75</t>
+  </si>
+  <si>
+    <t>[{"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"},{"internalType":"uint8","name":"_decimals","type":"uint8"},{"internalType":"address","name":"_owner","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"oldOwner","type":"address"},{"indexed":true,"internalType":"address","name":"newOwner","type":"address"},{"indexed":true,"internalType":"uint256","name":"effectiveTime","type":"uint256"}],"name":"LogChangeDCRMOwner","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"bytes32","name":"txhash","type":"bytes32"},{"indexed":true,"internalType":"address","name":"account","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"LogSwapin","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"account","type":"address"},{"indexed":true,"internalType":"address","name":"bindaddr","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"LogSwapout","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"bytes32","name":"txhash","type":"bytes32"},{"internalType":"address","name":"account","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Swapin","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"},{"internalType":"address","name":"bindaddr","type":"address"}],"name":"Swapout","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"TRANSFER_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"approveAndCall","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"newOwner","type":"address"}],"name":"changeDCRMOwner","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"owner","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"target","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"transferAndCall","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"target","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"transferWithPermit","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t>0xE3F5a90F9cb311505cd691a46596599aA1A0AD7D</t>
+  </si>
+  <si>
+    <t>[{"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"},{"internalType":"uint8","name":"_decimals","type":"uint8"},{"internalType":"address","name":"_underlying","type":"address"},{"internalType":"address","name":"_vault","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"auth","type":"address"},{"indexed":false,"internalType":"uint256","name":"timestamp","type":"uint256"}],"name":"LogAddAuth","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"oldOwner","type":"address"},{"indexed":true,"internalType":"address","name":"newOwner","type":"address"},{"indexed":true,"internalType":"uint256","name":"effectiveHeight","type":"uint256"}],"name":"LogChangeMPCOwner","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"oldVault","type":"address"},{"indexed":true,"internalType":"address","name":"newVault","type":"address"},{"indexed":true,"internalType":"uint256","name":"effectiveTime","type":"uint256"}],"name":"LogChangeVault","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"bytes32","name":"txhash","type":"bytes32"},{"indexed":true,"internalType":"address","name":"account","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"LogSwapin","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"account","type":"address"},{"indexed":true,"internalType":"address","name":"bindaddr","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"LogSwapout","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"bytes32","name":"txhash","type":"bytes32"},{"internalType":"address","name":"account","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Swapin","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"},{"internalType":"address","name":"bindaddr","type":"address"}],"name":"Swapout","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"TRANSFER_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"applyMinter","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"applyVault","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"approveAndCall","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"burn","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newVault","type":"address"}],"name":"changeMPCOwner","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newVault","type":"address"}],"name":"changeVault","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"delay","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"delayDelay","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"delayMinter","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"delayVault","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"},{"internalType":"address","name":"to","type":"address"}],"name":"deposit","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"deposit","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"deposit","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"},{"internalType":"address","name":"to","type":"address"}],"name":"depositVault","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"target","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"},{"internalType":"address","name":"to","type":"address"}],"name":"depositWithPermit","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"target","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"},{"internalType":"address","name":"to","type":"address"}],"name":"depositWithTransferPermit","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"getAllMinters","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_vault","type":"address"}],"name":"initVault","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"isMinter","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"minters","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"mpc","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"owner","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"pendingDelay","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"pendingMinter","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"pendingVault","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"target","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_auth","type":"address"}],"name":"revokeMinter","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_auth","type":"address"}],"name":"setMinter","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_vault","type":"address"}],"name":"setVault","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"bool","name":"enabled","type":"bool"}],"name":"setVaultOnly","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"transferAndCall","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"target","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"transferWithPermit","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"vault","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"},{"internalType":"address","name":"to","type":"address"}],"name":"withdraw","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"withdraw","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"withdraw","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"},{"internalType":"address","name":"to","type":"address"}],"name":"withdrawVault","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t>0xc21223249CA28397B4B6541dfFaEcC539BfF0c59</t>
+  </si>
+  <si>
+    <t>StablecoinTokenAddress</t>
+  </si>
+  <si>
+    <t>StablecoinTokenAbi</t>
+  </si>
+  <si>
+    <t>0xe9e7CEA3DedcA5984780Bafc599bD69ADd087D56</t>
+  </si>
+  <si>
+    <t>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"previousOwner","type":"address"},{"indexed":true,"internalType":"address","name":"newOwner","type":"address"}],"name":"OwnershipTransferred","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"_decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"_name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"_symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"burn","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"subtractedValue","type":"uint256"}],"name":"decreaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"getOwner","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"addedValue","type":"uint256"}],"name":"increaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"owner","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"renounceOwnership","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"sender","type":"address"},{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newOwner","type":"address"}],"name":"transferOwnership","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t>[{"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"},{"internalType":"address","name":"_creator_address","type":"address"},{"internalType":"uint256","name":"_initial_mint_amt","type":"uint256"},{"internalType":"address","name":"_custodian_address","type":"address"},{"internalType":"address[]","name":"_bridge_tokens","type":"address[]"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"bridge_token_address","type":"address"}],"name":"BridgeTokenAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"bridge_token_address","type":"address"},{"indexed":false,"internalType":"bool","name":"state","type":"bool"}],"name":"BridgeTokenToggled","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"global_collateral_ratio","type":"uint256"}],"name":"CollateralRatioRefreshed","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"custodian_address","type":"address"}],"name":"CustodianSet","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"new_mint_cap","type":"uint256"}],"name":"MintCapSet","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"pool_address","type":"address"}],"name":"MinterAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"pool_address","type":"address"}],"name":"MinterRemoved","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldOwner","type":"address"},{"indexed":false,"internalType":"address","name":"newOwner","type":"address"}],"name":"OwnerChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"newOwner","type":"address"}],"name":"OwnerNominated","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"new_timelock","type":"address"}],"name":"TimelockSet","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"TokenBurned","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"TokenMinted","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"acceptOwnership","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"bridge_token_address","type":"address"}],"name":"addBridgeToken","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"minter_address","type":"address"}],"name":"addMinter","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"allBridgeTokens","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"bridge_tokens","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"bridge_tokens_array","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"burn","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"burnFrom","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"canSwap","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"custodian_address","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"subtractedValue","type":"uint256"}],"name":"decreaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"bridge_token_address","type":"address"},{"internalType":"uint256","name":"token_amount","type":"uint256"}],"name":"exchangeCanonicalForOld","outputs":[{"internalType":"uint256","name":"bridge_tokens_out","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"bridge_token_address","type":"address"},{"internalType":"uint256","name":"token_amount","type":"uint256"}],"name":"exchangeOldForCanonical","outputs":[{"internalType":"uint256","name":"canonical_tokens_out","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"exchangesPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_to","type":"address"},{"internalType":"uint256","name":"_value","type":"uint256"},{"internalType":"bytes","name":"_data","type":"bytes"}],"name":"execute","outputs":[{"internalType":"bool","name":"","type":"bool"},{"internalType":"bytes","name":"","type":"bytes"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"fee_exempt_list","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"addedValue","type":"uint256"}],"name":"increaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"mint_cap","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"minter_burn","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"m_address","type":"address"},{"internalType":"uint256","name":"m_amount","type":"uint256"}],"name":"minter_mint","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"minters","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"minters_array","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_owner","type":"address"}],"name":"nominateNewOwner","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"nominatedOwner","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"owner","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"tokenAddress","type":"address"},{"internalType":"uint256","name":"tokenAmount","type":"uint256"}],"name":"recoverERC20","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"minter_address","type":"address"}],"name":"removeMinter","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_custodian_address","type":"address"}],"name":"setCustodian","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"_mint_cap","type":"uint256"}],"name":"setMintCap","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"bridge_token_address","type":"address"},{"internalType":"uint256","name":"_bridge_to_canonical","type":"uint256"},{"internalType":"uint256","name":"_canonical_to_old","type":"uint256"}],"name":"setSwapFees","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"new_timelock","type":"address"}],"name":"setTimelock","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"uint256","name":"","type":"uint256"}],"name":"swap_fees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"timelock_address","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"bridge_token_address","type":"address"}],"name":"toggleBridgeToken","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"toggleExchanges","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"the_address","type":"address"}],"name":"toggleFeesForAddress","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"sender","type":"address"},{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"bridge_token_address","type":"address"},{"internalType":"uint256","name":"bridge_token_amount","type":"uint256"}],"name":"withdrawBridgeTokens","outputs":[],"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t>0x5ce9F0B6AFb36135b5ddBF11705cEB65E634A9dC</t>
+  </si>
+  <si>
+    <t>USD Coin</t>
+  </si>
+  <si>
+    <t>USDC.e</t>
+  </si>
+  <si>
+    <t>USDC</t>
+  </si>
+  <si>
+    <t>0x2791bca1f2de4661ed88a30c99a7a9449aa84174</t>
+  </si>
+  <si>
+    <t>[{"inputs":[{"internalType":"address","name":"_proxyTo","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"_new","type":"address"},{"indexed":false,"internalType":"address","name":"_old","type":"address"}],"name":"ProxyOwnerUpdate","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"_new","type":"address"},{"indexed":true,"internalType":"address","name":"_old","type":"address"}],"name":"ProxyUpdated","type":"event"},{"stateMutability":"payable","type":"fallback"},{"inputs":[],"name":"IMPLEMENTATION_SLOT","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"OWNER_SLOT","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"proxyOwner","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"proxyType","outputs":[{"internalType":"uint256","name":"proxyTypeId","type":"uint256"}],"stateMutability":"pure","type":"function"},{"inputs":[{"internalType":"address","name":"newOwner","type":"address"}],"name":"transferProxyOwnership","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_newProxyTo","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"updateAndCall","outputs":[],"stateMutability":"payable","type":"function"},{"inputs":[{"internalType":"address","name":"_newProxyTo","type":"address"}],"name":"updateImplementation","outputs":[],"stateMutability":"nonpayable","type":"function"},{"stateMutability":"payable","type":"receive"}]</t>
+  </si>
+  <si>
+    <t>Binance USD</t>
+  </si>
+  <si>
+    <t>BUSD</t>
+  </si>
+  <si>
+    <t>StablecoinName</t>
+  </si>
+  <si>
+    <t>StablecoinSymbol</t>
+  </si>
+  <si>
+    <t>StablecoinDecimals</t>
+  </si>
+  <si>
+    <t>UST Terra</t>
+  </si>
+  <si>
+    <t>atUST</t>
+  </si>
+  <si>
+    <t>FactoryAddress</t>
+  </si>
+  <si>
+    <t>FactoryAddressAbi</t>
+  </si>
+  <si>
+    <t>0x049581aEB6Fe262727f290165C29BDAB065a1B68</t>
+  </si>
+  <si>
+    <t>[{"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"token0","type":"address"},{"indexed":true,"internalType":"address","name":"token1","type":"address"},{"indexed":false,"internalType":"address","name":"pair","type":"address"},{"indexed":false,"internalType":"uint256","name":"","type":"uint256"}],"name":"PairCreated","type":"event"},{"inputs":[],"name":"INIT_CODE_PAIR_HASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allPairs","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"allPairsLength","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"auro","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"tokenA","type":"address"},{"internalType":"address","name":"tokenB","type":"address"}],"name":"createPair","outputs":[{"internalType":"address","name":"pair","type":"address"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"pairAddress","type":"address"}],"name":"disableMetaTxnsPair","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"pairAddress","type":"address"}],"name":"enableMetaTxnsPair","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"feeTo","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"feeToSetter","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"getPair","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"migrator","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_auro","type":"address"}],"name":"setAuroAddress","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_feeTo","type":"address"}],"name":"setFeeTo","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"}],"name":"setFeeToSetter","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_migrator","type":"address"}],"name":"setMigrator","outputs":[],"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t>[{"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"token0","type":"address"},{"indexed":true,"internalType":"address","name":"token1","type":"address"},{"indexed":false,"internalType":"address","name":"pair","type":"address"},{"indexed":false,"internalType":"uint256","name":"","type":"uint256"}],"name":"PairCreated","type":"event"},{"constant":true,"inputs":[],"name":"INIT_CODE_PAIR_HASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allPairs","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"allPairsLength","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"tokenA","type":"address"},{"internalType":"address","name":"tokenB","type":"address"}],"name":"createPair","outputs":[{"internalType":"address","name":"pair","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"feeTo","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"feeToSetter","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"getPair","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_feeTo","type":"address"}],"name":"setFeeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"}],"name":"setFeeToSetter","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t>0xcA143Ce32Fe78f1f7019d7d551a6402fC5350c73</t>
+  </si>
+  <si>
+    <t>0x9Ad6C38BE94206cA50bb0d90783181662f0Cfa10</t>
+  </si>
+  <si>
+    <t>[{"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"token0","type":"address"},{"indexed":true,"internalType":"address","name":"token1","type":"address"},{"indexed":false,"internalType":"address","name":"pair","type":"address"},{"indexed":false,"internalType":"uint256","name":"","type":"uint256"}],"name":"PairCreated","type":"event"},{"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allPairs","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"allPairsLength","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"tokenA","type":"address"},{"internalType":"address","name":"tokenB","type":"address"}],"name":"createPair","outputs":[{"internalType":"address","name":"pair","type":"address"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"feeTo","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"feeToSetter","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"getPair","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"migrator","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"pairCodeHash","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"pure","type":"function"},{"inputs":[{"internalType":"address","name":"_feeTo","type":"address"}],"name":"setFeeTo","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"}],"name":"setFeeToSetter","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_migrator","type":"address"}],"name":"setMigrator","outputs":[],"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t>0xef45d134b73241eda7703fa787148d9c9f4950b0</t>
+  </si>
+  <si>
+    <t>[{"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"},{"internalType":"bool","name":"_locked","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"token0","type":"address"},{"indexed":true,"internalType":"address","name":"token1","type":"address"},{"indexed":false,"internalType":"address","name":"pair","type":"address"},{"indexed":false,"internalType":"uint256","name":"","type":"uint256"}],"name":"PairCreated","type":"event"},{"constant":true,"inputs":[],"name":"INIT_CODE_PAIR_HASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allPairs","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"allPairsLength","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"tokenA","type":"address"},{"internalType":"address","name":"tokenB","type":"address"}],"name":"createPair","outputs":[{"internalType":"address","name":"pair","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"feeTo","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"feeToSetter","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"getPair","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"locked","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_feeTo","type":"address"}],"name":"setFeeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"}],"name":"setFeeToSetter","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"_locked","type":"bool"}],"name":"setLocked","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t>0x152ee697f2e276fa89e96742e9bb9ab1f2e61be3</t>
+  </si>
+  <si>
+    <t>[{"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"token0","type":"address"},{"indexed":true,"internalType":"address","name":"token1","type":"address"},{"indexed":false,"internalType":"address","name":"pair","type":"address"},{"indexed":false,"internalType":"uint256","name":"","type":"uint256"}],"name":"PairCreated","type":"event"},{"inputs":[],"name":"INIT_CODE_PAIR_HASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allPairs","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"allPairsLength","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"tokenA","type":"address"},{"internalType":"address","name":"tokenB","type":"address"}],"name":"createPair","outputs":[{"internalType":"address","name":"pair","type":"address"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"feeTo","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"feeToSetter","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"getPair","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"pairCodeHash","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"pure","type":"function"},{"inputs":[{"internalType":"address","name":"_feeTo","type":"address"}],"name":"setFeeTo","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"}],"name":"setFeeToSetter","outputs":[],"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t>0x3b44b2a187a7b3824131f8db5a74194d0a42fc15</t>
+  </si>
+  <si>
+    <t>[{"type":"constructor","stateMutability":"nonpayable","payable":false,"inputs":[{"type":"address","name":"_feeToSetter","internalType":"address"}]},{"type":"event","name":"PairCreated","inputs":[{"type":"address","name":"token0","internalType":"address","indexed":true},{"type":"address","name":"token1","internalType":"address","indexed":true},{"type":"address","name":"pair","internalType":"address","indexed":false},{"type":"uint256","name":"","internalType":"uint256","indexed":false}],"anonymous":false},{"type":"function","stateMutability":"view","payable":false,"outputs":[{"type":"bytes32","name":"","internalType":"bytes32"}],"name":"INIT_CODE_PAIR_HASH","inputs":[],"constant":true},{"type":"function","stateMutability":"view","payable":false,"outputs":[{"type":"address","name":"","internalType":"address"}],"name":"allPairs","inputs":[{"type":"uint256","name":"","internalType":"uint256"}],"constant":true},{"type":"function","stateMutability":"view","payable":false,"outputs":[{"type":"uint256","name":"","internalType":"uint256"}],"name":"allPairsLength","inputs":[],"constant":true},{"type":"function","stateMutability":"nonpayable","payable":false,"outputs":[{"type":"address","name":"pair","internalType":"address"}],"name":"createPair","inputs":[{"type":"address","name":"tokenA","internalType":"address"},{"type":"address","name":"tokenB","internalType":"address"}],"constant":false},{"type":"function","stateMutability":"view","payable":false,"outputs":[{"type":"address","name":"","internalType":"address"}],"name":"feeTo","inputs":[],"constant":true},{"type":"function","stateMutability":"view","payable":false,"outputs":[{"type":"address","name":"","internalType":"address"}],"name":"feeToSetter","inputs":[],"constant":true},{"type":"function","stateMutability":"view","payable":false,"outputs":[{"type":"address","name":"","internalType":"address"}],"name":"getPair","inputs":[{"type":"address","name":"","internalType":"address"},{"type":"address","name":"","internalType":"address"}],"constant":true},{"type":"function","stateMutability":"nonpayable","payable":false,"outputs":[],"name":"setFeeTo","inputs":[{"type":"address","name":"_feeTo","internalType":"address"}],"constant":false},{"type":"function","stateMutability":"nonpayable","payable":false,"outputs":[],"name":"setFeeToSetter","inputs":[{"type":"address","name":"_feeToSetter","internalType":"address"}],"constant":false}]</t>
+  </si>
+  <si>
+    <t>0xc66F594268041dB60507F00703b152492fb176E7</t>
+  </si>
+  <si>
+    <t>[{"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"token0","type":"address"},{"indexed":true,"internalType":"address","name":"token1","type":"address"},{"indexed":false,"internalType":"address","name":"pair","type":"address"},{"indexed":false,"internalType":"uint256","name":"","type":"uint256"}],"name":"PairCreated","type":"event"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allPairs","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"allPairsLength","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"tokenA","type":"address"},{"internalType":"address","name":"tokenB","type":"address"}],"name":"createPair","outputs":[{"internalType":"address","name":"pair","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"feeTo","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"feeToSetter","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"getPair","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_feeTo","type":"address"}],"name":"setFeeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_feeToSetter","type":"address"}],"name":"setFeeToSetter","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t>0x5C69bEe701ef814a2B6a3EDD4B1652CB9cc5aA6f</t>
+  </si>
+  <si>
+    <t>Explorer</t>
+  </si>
+  <si>
+    <t>https://moonriver.moonscan.io/</t>
+  </si>
+  <si>
+    <t>https://ftmscan.com/</t>
+  </si>
+  <si>
+    <t>https://snowtrace.io/</t>
+  </si>
+  <si>
+    <t>https://bscscan.com/</t>
+  </si>
+  <si>
+    <t>https://cronos.crypto.org/explorer/</t>
+  </si>
+  <si>
+    <t>https://explorer.mainnet.aurora.dev/</t>
+  </si>
+  <si>
+    <t>https://polygonscan.com/</t>
   </si>
 </sst>
 </file>
@@ -553,10 +703,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88998168-CC66-D04F-A4D5-FDD2D1EEBC84}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,13 +717,21 @@
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="255.83203125" customWidth="1"/>
+    <col min="12" max="12" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -581,19 +742,43 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>35</v>
       </c>
+      <c r="N1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -603,20 +788,44 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="M2" t="s">
         <v>9</v>
       </c>
+      <c r="N2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -626,20 +835,44 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="M3" t="s">
         <v>16</v>
       </c>
+      <c r="N3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O3" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -649,20 +882,44 @@
       <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
+      <c r="M4" t="s">
         <v>9</v>
       </c>
+      <c r="N4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -672,20 +929,44 @@
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" t="s">
+      <c r="M5" t="s">
         <v>9</v>
       </c>
+      <c r="N5" t="s">
+        <v>88</v>
+      </c>
+      <c r="O5" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -695,20 +976,44 @@
       <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" t="s">
+      <c r="M6" t="s">
         <v>31</v>
       </c>
+      <c r="N6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O6" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -718,20 +1023,44 @@
       <c r="C7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" t="s">
         <v>39</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" t="s">
         <v>40</v>
       </c>
-      <c r="G7" t="s">
+      <c r="M7" t="s">
         <v>9</v>
       </c>
+      <c r="N7" t="s">
+        <v>94</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -741,21 +1070,44 @@
       <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" t="s">
         <v>45</v>
       </c>
-      <c r="G8" t="s">
+      <c r="M8" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="N8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -765,17 +1117,41 @@
       <c r="C9" t="s">
         <v>48</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" t="s">
         <v>49</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>50</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" t="s">
         <v>51</v>
       </c>
-      <c r="G9" t="s">
+      <c r="M9" t="s">
         <v>52</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -786,6 +1162,14 @@
     <hyperlink ref="C5" r:id="rId4" xr:uid="{9A227C98-F9AC-1048-9303-57A39C9856C3}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{F5F43F09-3564-9942-B1DA-80E21B44E1AB}"/>
     <hyperlink ref="C7" r:id="rId6" xr:uid="{18609CA7-5AA4-0E41-B8EB-45FCD244B03B}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{6123A671-3F14-3947-9FAA-9954349F2C2D}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{E2ED65B4-2D65-6D4F-9611-E9437C698614}"/>
+    <hyperlink ref="D4" r:id="rId9" xr:uid="{C25F3E10-5A97-474A-8302-171D6E12A068}"/>
+    <hyperlink ref="D3" r:id="rId10" xr:uid="{6C8593F4-E39C-7044-BAB4-116000ECB4E1}"/>
+    <hyperlink ref="D2" r:id="rId11" xr:uid="{D2ABED63-83FA-AA46-8685-A144C62D2069}"/>
+    <hyperlink ref="D9" r:id="rId12" xr:uid="{699E65F7-54AF-5445-BBA2-CA3429208577}"/>
+    <hyperlink ref="D8" r:id="rId13" xr:uid="{7406FDF9-A9F3-6B4E-ADAF-81CB163E94D8}"/>
+    <hyperlink ref="D7" r:id="rId14" xr:uid="{0155EACC-5915-2446-9A96-04B353907789}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>